<commit_message>
visits and cashflow generation
</commit_message>
<xml_diff>
--- a/generate/dogs.xlsx
+++ b/generate/dogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bogna Jaszczak\Desktop\bazy danych\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1f377440ec0e54a/Documents/vet_clinic/generate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60FDA798-D2C9-4C00-893F-9A04646ABEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{60FDA798-D2C9-4C00-893F-9A04646ABEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA12DDA-3508-44F5-9068-B5B558EC87B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dog" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>breed</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>Sussex Spaniel</t>
-  </si>
-  <si>
-    <t>Vizsla</t>
   </si>
   <si>
     <t>Welsh Springer Spaniel</t>
@@ -484,7 +481,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1336,11 +1333,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,21 +1354,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
         <v>149</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>150</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>151</v>
-      </c>
-      <c r="E1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>0.2286</v>
@@ -1439,7 +1436,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>0.2286</v>
@@ -1558,7 +1555,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13">
         <v>0.254</v>
@@ -1575,7 +1572,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14">
         <v>0.43179999999999996</v>
@@ -1609,7 +1606,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16">
         <v>0.33019999999999999</v>
@@ -1660,7 +1657,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19">
         <v>0.38100000000000001</v>
@@ -1745,7 +1742,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24">
         <v>0.24129999999999999</v>
@@ -1830,7 +1827,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29">
         <v>0.30479999999999996</v>
@@ -1864,7 +1861,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31">
         <v>0.35559999999999997</v>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B36">
         <v>0.17779999999999999</v>
@@ -2017,7 +2014,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40">
         <v>0.2286</v>
@@ -2051,7 +2048,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42">
         <v>0.254</v>
@@ -2068,7 +2065,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43">
         <v>0.254</v>
@@ -2102,7 +2099,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45">
         <v>0.15239999999999998</v>
@@ -2119,7 +2116,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46">
         <v>0.27939999999999998</v>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54">
         <v>0.17779999999999999</v>
@@ -2289,7 +2286,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B56">
         <v>0.4572</v>
@@ -2374,7 +2371,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61">
         <v>0.254</v>
@@ -2442,7 +2439,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65">
         <v>0.33019999999999999</v>
@@ -2459,7 +2456,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66">
         <v>0.33019999999999999</v>
@@ -2476,7 +2473,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B67">
         <v>0.27939999999999998</v>
@@ -2493,7 +2490,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B68">
         <v>0.40639999999999998</v>
@@ -2578,7 +2575,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B73">
         <v>0.35559999999999997</v>
@@ -2799,7 +2796,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B86">
         <v>0.30479999999999996</v>
@@ -2816,7 +2813,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B87">
         <v>0.20319999999999999</v>
@@ -2918,7 +2915,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B93">
         <v>0.33019999999999999</v>
@@ -2935,7 +2932,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B94">
         <v>0.20319999999999999</v>
@@ -2952,7 +2949,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B95">
         <v>0.38100000000000001</v>
@@ -2969,7 +2966,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96">
         <v>0.254</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B104">
         <v>0.20319999999999999</v>
@@ -3207,7 +3204,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B110">
         <v>0.30479999999999996</v>
@@ -3224,7 +3221,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B111">
         <v>0.254</v>
@@ -3258,7 +3255,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B113">
         <v>0.254</v>
@@ -3292,7 +3289,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B115">
         <v>0.254</v>
@@ -3309,7 +3306,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B116">
         <v>0.40639999999999998</v>
@@ -3428,7 +3425,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>0.254</v>
@@ -3462,7 +3459,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125">
         <v>0.254</v>
@@ -3479,7 +3476,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126">
         <v>0.30479999999999996</v>
@@ -3496,7 +3493,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127">
         <v>0.33019999999999999</v>
@@ -3513,7 +3510,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128">
         <v>0.33019999999999999</v>
@@ -3530,7 +3527,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B129">
         <v>0.20319999999999999</v>
@@ -3564,7 +3561,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>0.2286</v>
@@ -3581,7 +3578,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>0.254</v>
@@ -3700,7 +3697,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B139">
         <v>0.254</v>
@@ -3717,7 +3714,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B140">
         <v>0.35559999999999997</v>
@@ -3734,7 +3731,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B141">
         <v>0.254</v>
@@ -3751,53 +3748,53 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="B142">
-        <v>1.2191999999999998</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="C142">
-        <v>1.6763999999999999</v>
+        <v>0.68579999999999997</v>
       </c>
       <c r="D142">
-        <v>9.979032140000001</v>
+        <v>31.751465900000003</v>
       </c>
       <c r="E142">
-        <v>11.33980925</v>
+        <v>38.555351450000003</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B143">
-        <v>0.63500000000000001</v>
+        <v>0.40639999999999998</v>
       </c>
       <c r="C143">
-        <v>0.68579999999999997</v>
+        <v>0.48259999999999997</v>
       </c>
       <c r="D143">
-        <v>31.751465900000003</v>
+        <v>15.875732950000002</v>
       </c>
       <c r="E143">
-        <v>38.555351450000003</v>
+        <v>20.411656650000001</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="B144">
-        <v>0.40639999999999998</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="C144">
-        <v>0.48259999999999997</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="D144">
-        <v>15.875732950000002</v>
+        <v>9.0718474000000011</v>
       </c>
       <c r="E144">
-        <v>20.411656650000001</v>
+        <v>9.5254397700000002</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3805,16 +3802,16 @@
         <v>134</v>
       </c>
       <c r="B145">
-        <v>0.38100000000000001</v>
+        <v>0.27939999999999998</v>
       </c>
       <c r="C145">
-        <v>0.38100000000000001</v>
+        <v>0.27939999999999998</v>
       </c>
       <c r="D145">
-        <v>9.0718474000000011</v>
+        <v>5.8967008100000005</v>
       </c>
       <c r="E145">
-        <v>9.5254397700000002</v>
+        <v>6.8038855500000004</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3822,66 +3819,49 @@
         <v>135</v>
       </c>
       <c r="B146">
-        <v>0.27939999999999998</v>
+        <v>0.4572</v>
       </c>
       <c r="C146">
-        <v>0.27939999999999998</v>
+        <v>0.55879999999999996</v>
       </c>
       <c r="D146">
-        <v>5.8967008100000005</v>
+        <v>12.24699399</v>
       </c>
       <c r="E146">
-        <v>6.8038855500000004</v>
+        <v>13.607771100000001</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="B147">
-        <v>0.4572</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C147">
-        <v>0.55879999999999996</v>
+        <v>0.60959999999999992</v>
       </c>
       <c r="D147">
-        <v>12.24699399</v>
+        <v>20.411656650000001</v>
       </c>
       <c r="E147">
-        <v>13.607771100000001</v>
+        <v>27.215542200000002</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B148">
-        <v>0.50800000000000001</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="C148">
-        <v>0.60959999999999992</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="D148">
-        <v>20.411656650000001</v>
+        <v>1.3607771100000001</v>
       </c>
       <c r="E148">
-        <v>27.215542200000002</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>148</v>
-      </c>
-      <c r="B149">
-        <v>0.20319999999999999</v>
-      </c>
-      <c r="C149">
-        <v>0.20319999999999999</v>
-      </c>
-      <c r="D149">
-        <v>1.3607771100000001</v>
-      </c>
-      <c r="E149">
         <v>3.1751465900000002</v>
       </c>
     </row>

</xml_diff>